<commit_message>
Ammedment : dynamic function to update parameters based on user input freature to have default value Vs user defined parameteres
</commit_message>
<xml_diff>
--- a/www/Persona_share.xlsx
+++ b/www/Persona_share.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slakshminarayanan\Desktop\Reckitt_shiny_app\code\V1\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF14870-8FB5-448F-86EE-7B97B8557FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76594530-8C2A-4653-80AC-A203D3CB3345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,6 +114,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.00000000E+00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,11 +160,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,16 +449,19 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.08984375" customWidth="1"/>
     <col min="10" max="17" width="15.90625" customWidth="1"/>
-    <col min="18" max="18" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -742,8 +749,8 @@
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5">
-        <f t="shared" si="1"/>
+      <c r="R5" s="4">
+        <f>1/((B5*J5*N5*F5)+(C5*K5*O5*G5)+(D5*L5*P5*H5)+(E5*M5*Q5*I5))</f>
         <v>3.2912058978409687E-5</v>
       </c>
     </row>

</xml_diff>